<commit_message>
Added the few articles in PZ
</commit_message>
<xml_diff>
--- a/Формуляр расчета баллов по КП.xlsx
+++ b/Формуляр расчета баллов по КП.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YaBer\Downloads\Telegram Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Study\4 course\Practice\OBD\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="41">
   <si>
     <t>Введение</t>
   </si>
@@ -141,6 +141,9 @@
   </si>
   <si>
     <t>+</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -696,7 +699,7 @@
   <dimension ref="B2:N41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -745,6 +748,9 @@
         <f>SUM(L4)</f>
         <v>10</v>
       </c>
+      <c r="N3" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" s="9"/>
@@ -763,6 +769,9 @@
         <v>10</v>
       </c>
       <c r="M4" s="16"/>
+      <c r="N4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="8">
@@ -805,6 +814,9 @@
         <v>2</v>
       </c>
       <c r="M6" s="17"/>
+      <c r="N6" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" s="10"/>
@@ -865,6 +877,9 @@
         <v>3</v>
       </c>
       <c r="M9" s="17"/>
+      <c r="N9" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" s="9"/>
@@ -928,6 +943,9 @@
         <v>5</v>
       </c>
       <c r="M12" s="17"/>
+      <c r="N12" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13" s="10"/>
@@ -1030,6 +1048,9 @@
         <v>10</v>
       </c>
       <c r="M17" s="17"/>
+      <c r="N17" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18" s="10"/>
@@ -1048,6 +1069,9 @@
         <v>3</v>
       </c>
       <c r="M18" s="17"/>
+      <c r="N18" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B19" s="9"/>

</xml_diff>